<commit_message>
add FP-Growth manual calculation
</commit_message>
<xml_diff>
--- a/SEMPRO/Data Penjualan Shehrazat.id Shopee 14 Feb - 14 Mar.xlsx
+++ b/SEMPRO/Data Penjualan Shehrazat.id Shopee 14 Feb - 14 Mar.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2025" yWindow="15" windowWidth="18450" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="2025" yWindow="15" windowWidth="18450" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Data Clean" sheetId="1" r:id="rId1"/>
@@ -1018,12 +1018,6 @@
     <xf numFmtId="10" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1032,6 +1026,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1372,8 +1372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D131"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="C102" sqref="C102"/>
+    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="C133" sqref="C133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2422,8 +2422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AQ26" sqref="AQ26"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2458,63 +2458,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="D1" s="29" t="s">
+      <c r="B1" s="32"/>
+      <c r="D1" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="H1" s="29" t="s">
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="H1" s="33" t="s">
         <v>221</v>
       </c>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="L1" s="29" t="s">
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="L1" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="P1" s="29" t="s">
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="P1" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="T1" s="28" t="s">
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="T1" s="32" t="s">
         <v>158</v>
       </c>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
-      <c r="AE1" s="28" t="s">
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="32"/>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AE1" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="AF1" s="28"/>
-      <c r="AH1" s="28" t="s">
+      <c r="AF1" s="32"/>
+      <c r="AH1" s="32" t="s">
         <v>198</v>
       </c>
-      <c r="AI1" s="28"/>
-      <c r="AK1" s="28" t="s">
+      <c r="AI1" s="32"/>
+      <c r="AK1" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="AL1" s="28"/>
-      <c r="AN1" s="28" t="s">
+      <c r="AL1" s="32"/>
+      <c r="AN1" s="32" t="s">
         <v>173</v>
       </c>
-      <c r="AO1" s="28"/>
-      <c r="AQ1" s="28" t="s">
+      <c r="AO1" s="32"/>
+      <c r="AQ1" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="AR1" s="28"/>
-      <c r="AS1" s="28"/>
+      <c r="AR1" s="32"/>
+      <c r="AS1" s="32"/>
     </row>
     <row r="2" spans="1:45" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -3027,7 +3027,7 @@
       <c r="AH8" s="9">
         <v>3</v>
       </c>
-      <c r="AI8" s="31" t="s">
+      <c r="AI8" s="29" t="s">
         <v>235</v>
       </c>
       <c r="AK8" s="9">
@@ -3846,7 +3846,7 @@
         <f>3/25*100</f>
         <v>12</v>
       </c>
-      <c r="AS21" s="32">
+      <c r="AS21" s="30">
         <f>3/3*100</f>
         <v>100</v>
       </c>
@@ -3956,13 +3956,13 @@
       <c r="AO23" s="21" t="s">
         <v>254</v>
       </c>
-      <c r="AQ23" s="32" t="s">
+      <c r="AQ23" s="30" t="s">
         <v>255</v>
       </c>
-      <c r="AR23" s="32">
+      <c r="AR23" s="30">
         <v>12</v>
       </c>
-      <c r="AS23" s="32">
+      <c r="AS23" s="30">
         <f>3/3*100</f>
         <v>100</v>
       </c>
@@ -4070,14 +4070,14 @@
       <c r="AO25" s="21" t="s">
         <v>257</v>
       </c>
-      <c r="AQ25" s="32" t="s">
+      <c r="AQ25" s="30" t="s">
         <v>259</v>
       </c>
-      <c r="AR25" s="32">
-        <f>3/25*100</f>
+      <c r="AR25" s="30">
+        <f t="shared" ref="AR25:AR32" si="2">3/25*100</f>
         <v>12</v>
       </c>
-      <c r="AS25" s="32">
+      <c r="AS25" s="30">
         <f>3/3*100</f>
         <v>100</v>
       </c>
@@ -4131,7 +4131,7 @@
         <v>260</v>
       </c>
       <c r="AR26" s="18">
-        <f>3/25*100</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="AS26" s="18">
@@ -4184,14 +4184,14 @@
       <c r="AO27" s="21" t="s">
         <v>262</v>
       </c>
-      <c r="AQ27" s="33" t="s">
+      <c r="AQ27" s="31" t="s">
         <v>263</v>
       </c>
-      <c r="AR27" s="33">
-        <f>3/25*100</f>
+      <c r="AR27" s="31">
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="AS27" s="33">
+      <c r="AS27" s="31">
         <f>3/3*100</f>
         <v>100</v>
       </c>
@@ -4227,7 +4227,7 @@
         <v>264</v>
       </c>
       <c r="AR28" s="18">
-        <f>3/25*100</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="AS28" s="18">
@@ -4268,7 +4268,7 @@
         <v>237</v>
       </c>
       <c r="AR29" s="18">
-        <f>3/25*100</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="AS29" s="18">
@@ -4303,14 +4303,14 @@
       <c r="AO30" s="21" t="s">
         <v>241</v>
       </c>
-      <c r="AQ30" s="32" t="s">
+      <c r="AQ30" s="30" t="s">
         <v>238</v>
       </c>
-      <c r="AR30" s="32">
-        <f>3/25*100</f>
+      <c r="AR30" s="30">
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="AS30" s="32">
+      <c r="AS30" s="30">
         <f>3/3*100</f>
         <v>100</v>
       </c>
@@ -4348,7 +4348,7 @@
         <v>244</v>
       </c>
       <c r="AR31" s="18">
-        <f>3/25*100</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="AS31" s="18">
@@ -4387,14 +4387,14 @@
       <c r="AO32" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="AQ32" s="32" t="s">
+      <c r="AQ32" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="AR32" s="32">
-        <f>3/25*100</f>
+      <c r="AR32" s="30">
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="AS32" s="32">
+      <c r="AS32" s="30">
         <f>3/4*100</f>
         <v>75</v>
       </c>
@@ -5114,17 +5114,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="AH1:AI1"/>
+    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="AN1:AO1"/>
+    <mergeCell ref="AQ1:AS1"/>
     <mergeCell ref="T1:AC1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="P1:R1"/>
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="AH1:AI1"/>
-    <mergeCell ref="AK1:AL1"/>
-    <mergeCell ref="AN1:AO1"/>
-    <mergeCell ref="AQ1:AS1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5155,7 +5155,7 @@
       <c r="N4" t="s">
         <v>222</v>
       </c>
-      <c r="O4" s="30" t="s">
+      <c r="O4" s="28" t="s">
         <v>224</v>
       </c>
       <c r="P4" t="s">
@@ -5175,7 +5175,7 @@
       <c r="N5" t="s">
         <v>222</v>
       </c>
-      <c r="O5" s="30" t="s">
+      <c r="O5" s="28" t="s">
         <v>225</v>
       </c>
       <c r="P5" t="s">
@@ -5195,7 +5195,7 @@
       <c r="N6" t="s">
         <v>222</v>
       </c>
-      <c r="O6" s="30" t="s">
+      <c r="O6" s="28" t="s">
         <v>226</v>
       </c>
       <c r="P6" t="s">
@@ -5215,7 +5215,7 @@
       <c r="N7" t="s">
         <v>222</v>
       </c>
-      <c r="O7" s="30" t="s">
+      <c r="O7" s="28" t="s">
         <v>227</v>
       </c>
       <c r="P7" t="s">
@@ -5235,7 +5235,7 @@
       <c r="N8" t="s">
         <v>222</v>
       </c>
-      <c r="O8" s="30" t="s">
+      <c r="O8" s="28" t="s">
         <v>228</v>
       </c>
       <c r="P8" t="s">
@@ -5255,7 +5255,7 @@
       <c r="N9" t="s">
         <v>222</v>
       </c>
-      <c r="O9" s="30" t="s">
+      <c r="O9" s="28" t="s">
         <v>229</v>
       </c>
       <c r="P9" t="s">
@@ -5275,7 +5275,7 @@
       <c r="N10" t="s">
         <v>222</v>
       </c>
-      <c r="O10" s="30" t="s">
+      <c r="O10" s="28" t="s">
         <v>230</v>
       </c>
       <c r="P10" t="s">
@@ -5295,7 +5295,7 @@
       <c r="N11" t="s">
         <v>222</v>
       </c>
-      <c r="O11" s="30" t="s">
+      <c r="O11" s="28" t="s">
         <v>231</v>
       </c>
       <c r="P11" t="s">
@@ -5315,7 +5315,7 @@
       <c r="N12" t="s">
         <v>222</v>
       </c>
-      <c r="O12" s="30" t="s">
+      <c r="O12" s="28" t="s">
         <v>232</v>
       </c>
       <c r="P12" t="s">
@@ -5335,7 +5335,7 @@
       <c r="N13" t="s">
         <v>222</v>
       </c>
-      <c r="O13" s="30" t="s">
+      <c r="O13" s="28" t="s">
         <v>233</v>
       </c>
       <c r="P13" t="s">

</xml_diff>

<commit_message>
add lift ratio calculation
</commit_message>
<xml_diff>
--- a/SEMPRO/Data Penjualan Shehrazat.id Shopee 14 Feb - 14 Mar.xlsx
+++ b/SEMPRO/Data Penjualan Shehrazat.id Shopee 14 Feb - 14 Mar.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2025" yWindow="15" windowWidth="18450" windowHeight="7995"/>
+    <workbookView xWindow="2025" yWindow="15" windowWidth="18450" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data Clean" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="271">
   <si>
     <t>No Pesanan</t>
   </si>
@@ -842,6 +842,9 @@
   </si>
   <si>
     <t>1 -&gt; 15, 14</t>
+  </si>
+  <si>
+    <t>Lift Ratio</t>
   </si>
 </sst>
 </file>
@@ -945,7 +948,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1033,6 +1036,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1372,7 +1378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
+    <sheetView topLeftCell="A114" workbookViewId="0">
       <selection activeCell="C133" sqref="C133"/>
     </sheetView>
   </sheetViews>
@@ -2420,10 +2426,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AS157"/>
+  <dimension ref="A1:AT157"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" topLeftCell="AO5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AW24" sqref="AW24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2457,7 +2463,7 @@
     <col min="45" max="45" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
         <v>106</v>
       </c>
@@ -2516,7 +2522,7 @@
       <c r="AR1" s="32"/>
       <c r="AS1" s="32"/>
     </row>
-    <row r="2" spans="1:45" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>119</v>
       </c>
@@ -2593,8 +2599,11 @@
       <c r="AS2" s="11" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT2" s="11" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>1</v>
       </c>
@@ -2674,8 +2683,11 @@
         <f>4/I17</f>
         <v>0.8</v>
       </c>
-    </row>
-    <row r="4" spans="1:45" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AT3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:46" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>2</v>
       </c>
@@ -2748,8 +2760,9 @@
         <f>4/I3</f>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="5" spans="1:45" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AT4" s="34"/>
+    </row>
+    <row r="5" spans="1:46" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>3</v>
       </c>
@@ -2823,8 +2836,12 @@
         <f>3/I17*100</f>
         <v>60</v>
       </c>
-    </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT5" s="2">
+        <f>60/24</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>4</v>
       </c>
@@ -2898,8 +2915,9 @@
         <f>3/I16*100</f>
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT6" s="34"/>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>5</v>
       </c>
@@ -2976,8 +2994,12 @@
         <f>3/3*100</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT7" s="2">
+        <f>100/80</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>6</v>
       </c>
@@ -3050,8 +3072,9 @@
         <f>3/20*100</f>
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT8" s="34"/>
+    </row>
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>7</v>
       </c>
@@ -3127,8 +3150,12 @@
         <f>4/I16</f>
         <v>0.66666666666666663</v>
       </c>
-    </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT9" s="34">
+        <f>66.67/80</f>
+        <v>0.83337499999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>8</v>
       </c>
@@ -3193,8 +3220,9 @@
         <f>4/I3*100</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT10" s="34"/>
+    </row>
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>9</v>
       </c>
@@ -3258,8 +3286,12 @@
         <f>5/I7*100</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT11" s="34">
+        <f>100/80</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>10</v>
       </c>
@@ -3325,8 +3357,9 @@
         <f>5/I3*100</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT12" s="34"/>
+    </row>
+    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>11</v>
       </c>
@@ -3390,8 +3423,12 @@
         <f>4/I24*100</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT13" s="34">
+        <f>100/80</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>12</v>
       </c>
@@ -3447,8 +3484,9 @@
         <f>4/I3*100</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT14" s="34"/>
+    </row>
+    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>13</v>
       </c>
@@ -3508,8 +3546,12 @@
         <f>3/I15*100</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT15" s="34">
+        <f>100/80</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>14</v>
       </c>
@@ -3565,8 +3607,9 @@
         <f>3/20*100</f>
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT16" s="34"/>
+    </row>
+    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>15</v>
       </c>
@@ -3622,8 +3665,12 @@
         <f>3/I15*100</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT17" s="34">
+        <f>100/24</f>
+        <v>4.166666666666667</v>
+      </c>
+    </row>
+    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>16</v>
       </c>
@@ -3679,8 +3726,9 @@
         <f>3/I16*100</f>
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT18" s="34"/>
+    </row>
+    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>17</v>
       </c>
@@ -3736,8 +3784,12 @@
         <f>3/I15*100</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT19" s="34">
+        <f>100/20</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>18</v>
       </c>
@@ -3793,8 +3845,12 @@
         <f>3/I17*100</f>
         <v>60</v>
       </c>
-    </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT20" s="34">
+        <f>60/12</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>19</v>
       </c>
@@ -3850,8 +3906,12 @@
         <f>3/3*100</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT21" s="34">
+        <f>100/80</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>20</v>
       </c>
@@ -3906,8 +3966,9 @@
         <f>3/20*100</f>
         <v>15</v>
       </c>
-    </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT22" s="34"/>
+    </row>
+    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>21</v>
       </c>
@@ -3966,8 +4027,12 @@
         <f>3/3*100</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT23" s="34">
+        <f>100/80</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>22</v>
       </c>
@@ -4022,8 +4087,9 @@
         <f>3/20*100</f>
         <v>15</v>
       </c>
-    </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT24" s="34"/>
+    </row>
+    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>23</v>
       </c>
@@ -4081,8 +4147,12 @@
         <f>3/3*100</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="26" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT25" s="34">
+        <f>100/24</f>
+        <v>4.166666666666667</v>
+      </c>
+    </row>
+    <row r="26" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>24</v>
       </c>
@@ -4138,8 +4208,9 @@
         <f>3/6*100</f>
         <v>50</v>
       </c>
-    </row>
-    <row r="27" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT26" s="34"/>
+    </row>
+    <row r="27" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>25</v>
       </c>
@@ -4195,8 +4266,12 @@
         <f>3/3*100</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="28" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT27" s="34">
+        <f>100/80</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>26</v>
       </c>
@@ -4234,8 +4309,9 @@
         <f>3/20*100</f>
         <v>15</v>
       </c>
-    </row>
-    <row r="29" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT28" s="34"/>
+    </row>
+    <row r="29" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <v>27</v>
       </c>
@@ -4275,8 +4351,9 @@
         <f>3/20*100</f>
         <v>15</v>
       </c>
-    </row>
-    <row r="30" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT29" s="34"/>
+    </row>
+    <row r="30" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>28</v>
       </c>
@@ -4314,8 +4391,12 @@
         <f>3/3*100</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="31" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT30" s="34">
+        <f>100/80</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>29</v>
       </c>
@@ -4355,8 +4436,9 @@
         <f>4/20*100</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="32" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT31" s="34"/>
+    </row>
+    <row r="32" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>30</v>
       </c>
@@ -4397,6 +4479,10 @@
       <c r="AS32" s="30">
         <f>3/4*100</f>
         <v>75</v>
+      </c>
+      <c r="AT32" s="34">
+        <f>75/80</f>
+        <v>0.9375</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -5114,17 +5200,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="AH1:AI1"/>
-    <mergeCell ref="AK1:AL1"/>
-    <mergeCell ref="AN1:AO1"/>
-    <mergeCell ref="AQ1:AS1"/>
     <mergeCell ref="T1:AC1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="P1:R1"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="AH1:AI1"/>
+    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="AN1:AO1"/>
+    <mergeCell ref="AQ1:AS1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>